<commit_message>
update: migration from tag to special, variables now have specification in their specific columns
</commit_message>
<xml_diff>
--- a/test/sample.xlsx
+++ b/test/sample.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\exam_builder\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F384A4-1DAF-402E-A6A4-0984EACB8885}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8247AB26-0584-4D38-AE26-7B95EE99767E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="QuestionSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Explanation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>question</t>
   </si>
@@ -45,19 +46,520 @@
     <t>correct_id</t>
   </si>
   <si>
-    <t>Test question A</t>
-  </si>
-  <si>
-    <t>Test question B</t>
+    <t>\[ x \]</t>
+  </si>
+  <si>
+    <t>$$ y $$</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>Test DynamicKey {alpha_0}{alpha_1}</t>
+  </si>
+  <si>
+    <t>{alpha_0}</t>
+  </si>
+  <si>
+    <t>{alpha_1}</t>
+  </si>
+  <si>
+    <t>Neither</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>{x}{y}|||Test FixedEquation by division {x} / {y} =</t>
+  </si>
+  <si>
+    <t>{x/y}</t>
+  </si>
+  <si>
+    <t>{y/x}</t>
+  </si>
+  <si>
+    <t>{x*y}</t>
+  </si>
+  <si>
+    <t>{1/x/y}</t>
+  </si>
+  <si>
+    <t>{x}{y}|||Test SingleEquation (4 * {x} + 3 * {y}) =</t>
+  </si>
+  <si>
+    <t>{4*x+3*y}</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>Test MathJax \( x^2 + y^2 = z^2 \)</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>is_multiple_choice</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t>is_dynamic_key</t>
+  </si>
+  <si>
+    <t>is_single_equation</t>
+  </si>
+  <si>
+    <t>is_fixed_equation</t>
+  </si>
+  <si>
+    <t>variable_limitation</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>The id of the correct answer (1-4). In case of multiple answer (is_multiple_choice), write them separated by a comma</t>
+  </si>
+  <si>
+    <t>1, 4</t>
+  </si>
+  <si>
+    <t>Sinh</t>
+  </si>
+  <si>
+    <t>Tin</t>
+  </si>
+  <si>
+    <t>A single mutually exclusive tag (questions of different category should NOT belong to the same questionnaire)</t>
+  </si>
+  <si>
+    <t>Multiple inclusive tag (questions of different tag can belong to the same questionnaire</t>
+  </si>
+  <si>
+    <t>g8_midterm</t>
+  </si>
+  <si>
+    <t>Define the type of the question. Can use: is_multiple_choice, is_dynamic_key, is_single_equation, is_fixed_equation
+is_fixed_equation and is_single_equation are mutually exclusive</t>
+  </si>
+  <si>
+    <t>Table Column</t>
+  </si>
+  <si>
+    <t>Test Single Equation v2 (with variable limitation) Prime {x} &amp; Non-Square {y}</t>
+  </si>
+  <si>
+    <t>{2*x+y}</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>x: [2, 10] prime
+y: [4, 36] nonsquare</t>
+  </si>
+  <si>
+    <t>Test Fixed Equation v2 (with variable limitation) \(x\) in [3, 9] and \(y\) Non-Prime in [2, 12]</t>
+  </si>
+  <si>
+    <t>x={x}</t>
+  </si>
+  <si>
+    <t>y={y}</t>
+  </si>
+  <si>
+    <t>x*y={x*y}</t>
+  </si>
+  <si>
+    <t>x%y={x%y}</t>
+  </si>
+  <si>
+    <t>x: [3, 9]
+y: [2, 12] nonprime</t>
+  </si>
+  <si>
+    <t>Special question type</t>
+  </si>
+  <si>
+    <t>Guide</t>
+  </si>
+  <si>
+    <t>Enable multiple choice option. When specifying multiple answer, separate them with comma. Other restrictions still apply</t>
+  </si>
+  <si>
+    <t>Support upto 10 different alphabetical key. Each {alpha_n} will be replaced with a randomized, consistent uppercase alphabetical character.
+E.g  {alpha_0}{alpha_1}{alpha_2} has {alpha_0}{alpha_1} as longest edge -&gt; will be substitute with something like AVD, AV</t>
+  </si>
+  <si>
+    <t>x: [2, 20] prime</t>
+  </si>
+  <si>
+    <t>x1: prime
+x2: [1, 18] square</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Used and required to specify variable type for is_fixed_equation &amp; is_single_equation.
+Format should be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>variable_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>spec1 spec2 …</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, for each variable, separated by endline. Spec can be:
+- range: denoted as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[start, end]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, variable will be created within this range (do contain start &amp; end)
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prime/nonprime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: when denoted, only use prime/not-prime value
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>square/nonsquare</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: when denoted, only use square/not-square value
+TODO: support </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>coprime, negrange</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> option</t>
+    </r>
+  </si>
+  <si>
+    <t>Same as is_fixed_equation; except that it only contains the correct answer at answer1. answer2-4 will be ignored, correct_id must be 1 (also ignored, but still need a value).
+Upon question generation, create 4 problems with identical choices but different correct answer.</t>
+  </si>
+  <si>
+    <t>g5_s1, hard, ssu</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Support variable based problem generator. Variables should be listed in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>variable_limitation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section in format </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>variable_name: spec1 spec 2 …</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and separated by endline</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Variables will be generated dynamically using spec. All expressions in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>question</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>answer1-4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> must be surrounded by curly bracket and only use the valid variables specified to calculate its expression
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Deprecated: append </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{variable_name1}{variable_name2}...|||</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the question; this will create variables in range [1, 0] and allow evaluating all expressions as noted.</t>
+    </r>
+  </si>
+  <si>
+    <t>Example2</t>
+  </si>
+  <si>
+    <t>Answer no. 1, necessary in all cases. Can use MathJax and embedded image/graph to beautify the looks.</t>
+  </si>
+  <si>
+    <t>Answer no. 2, necessary when not is_single_equation. Can use MathJax and embedded image/graph to beautify the looks.</t>
+  </si>
+  <si>
+    <t>Answer no. 3, necessary when not is_single_equation. Can use MathJax and embedded image/graph to beautify the looks.</t>
+  </si>
+  <si>
+    <t>Answer no. 4, necessary when not is_single_equation. Can use MathJax and embedded image/graph to beautify the looks.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Text of the question. Can use MathJax and embedded image/graph to beautify the looks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deprecated: For the problem that involve dynamic variable (is_single_equation, is_fixed_equation), must list the variables beforehand.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -84,13 +586,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -101,6 +645,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B41BAFDF-9127-4F38-ABC3-6489FE9E1C50}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0">
+  <autoFilter ref="A1:D11" xr:uid="{762BAE9A-CDAC-4D53-9762-A38BEB2C0CB0}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C66E66B1-6D34-4594-A496-12326AB54944}" name="Table Column" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{AD289239-88A0-4B73-83C8-7316225B98D5}" name="Meaning" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{184D5377-5E65-4FB0-A42A-4C38B233B86C}" name="Example"/>
+    <tableColumn id="4" xr3:uid="{A9BFA7F4-67CB-4E3E-B25A-4DC9F0F30F20}" name="Example2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CE110FE0-2F59-4158-BD77-054CCC9A57AF}" name="Table2" displayName="Table2" ref="A13:B17" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A13:B17" xr:uid="{5F9E2083-6A74-48C2-AEF7-D86DE9D24C39}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{8F4578EE-C387-4044-A222-873007CB8B35}" name="Special question type" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{3904FAFA-674B-4DF0-BCB7-EE499E063446}" name="Guide" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,75 +934,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="1">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
+      <c r="G7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143307A4-3C9B-4AFA-B3F3-E623FFD46CF5}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="128" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update: recalling data from remote
</commit_message>
<xml_diff>
--- a/test/sample.xlsx
+++ b/test/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="QuestionSheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuestionSheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1442,6 +1442,4711 @@
 w: [3, 10]</t>
         </is>
       </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Phân chia nhân trong quá trình nguyên phân thực chất là</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>phân chia các gene nằm ở ti thể.</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>phân chia vật chất di truyền DNA và nhiễm sắc thể.</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>phân chia các bào quan.</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>phân chia vật chất di truyền ở tế bào chất.</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Loại tế bào có thể phân chia và biệt hóa thành mọi tế bào của cơ thể trưởng thành gọi là</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>tế bào soma.</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>tế bào mô sẹo.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>tế bào gốc trưởng thành.</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>tế bào gốc phôi.</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>4</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Vi sinh vật nào sau đây được xếp vào nhóm vi sinh vật nhân sơ?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Nấm đơn bào.</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Vi nấm.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Tảo đơn bào.</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Vi khuẩn.</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>4</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Loài vi sinh vật có khả năng tổng hợp glucose theo con đường quang hợp là</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>vi khuẩn màu lục.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>vi khuẩn lam.</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>vi khuẩn màu tía.</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>vi khuẩn nitrate.</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Phát biểu nào dưới đây là đúng khi nói về quá trình phân bào?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Kì giữa là kì dài nhất trong các kì của nguyên phân.</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Ở kì giữa của giảm phân I, mỗi nhiễm sắc thể kép chỉ đính với vi ống ở một phía của tâm động.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Các nhiễm sắc thể tương đồng có thể trao đổi đoạn cho nhau (trao đổi chéo) tại kì giữa của giảm phân I.</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Trong giảm phân, sau mỗi lần phân bào, nhiễm sắc thể đều phải nhân đôi.</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Điểm khác biệt của tế bào gốc phôi so với tế bào gốc trưởng thành là</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>có nguồn gốc từ các mô của cơ thể trưởng thành.</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>có nguồn gốc từ khối tế bào mầm phôi của phôi nang.</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>chỉ có thể biệt hóa thành một số loại tế bào nhất định của cơ thể.</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>chỉ có khả năng phân chia trong khoảng thời gian trước khi cơ thể trưởng thành.</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Sản xuất thuốc kháng sinh là một ứng dụng của công nghệ vi sinh vật trong lĩnh vực</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>nông nghiệp.</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>thực phẩm.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>y dược.</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>xử lí chất thải.</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>3</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Việc ứng dụng vi sinh vật trong sản xuất nước tương, nước mắm dựa trên cơ sở khoa học chủ yếu nào sau đây?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Vi sinh vật có sự đa dạng về di truyền.</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Vi sinh vật có phổ sinh thái và dinh dưỡng rộng.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Vi sinh vật có khả năng phân giải các chất nhanh.</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Vi sinh vật có khả năngsinh trưởng nhanh, sinh sản mạnh.</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Vai trò nào sau đây không phải là vai trò của vi sinh vật đối với tự nhiên?</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Phân giải các chất thải và xác sinh vật thành chất khoáng.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Tạo ra O2 và chất dinh dưỡng cung cấp cho các sinh vật dị dưỡng.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Cộng sinh với nhiều loài sinh vật để đảm bảo sự tồn tại và phát triển của loài đó.</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Ứng dụng trong chế biến thực phẩm, sản xuất thuốc kháng sinh, vitamin.</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>4</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ưu điểm của thuốc trừ sâu sinh học so với thuốc trừ sâu hóa học là</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>có tác dụng nhanh chóng.</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>không gây ô nhiễm môi trường.</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>có khả năng diệt trừ sâu bệnh.</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>có khả năng cải tạo đất trồng.</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Cơ sở khoa học của việc sử dụng vi sinh vật trong xử lí ô nhiễm môi trường là</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>vi sinh vật có khả năng vận chuyển chất thải, chất độc hại và kim loại nặng xuống tầng sâu của địa chất.</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>vi sinh vật có khả năng sinh nhiệt để đốt cháy tất cả các chất thải, chất độc hại và kim loại nặng.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>vi sinh vật có khả năng tạo ra màng sinh học ngăn chặn chất thải, chất độc hại và kim loại nặng gây hại cho môi trường.</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>vi sinh vật có khả năng hấp thụ và phân giải chất thải, chất độc hại và kim loại nặng.</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>4</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Sản phẩm nào sau đây không phải là sản phẩm của công nghệ vi sinh vật?</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Sữa chua.</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Vaccine.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Chất kháng sinh.</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Lúa mì.</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>4</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Chủng vi sinh vật được ứng dụng trong sản xuất thuốc trừ sâu sinh học là</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Saccharomyces cerevisiae.</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Streptomyces griseus.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Bacillus thuringiensis.</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Rhizobium.</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>3</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Những biểu hiện nào sau đây chứng tỏ kết quả làm sữa chua đã thành công?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Sữa chua đông tụ, có màu trắng sữa, có vị chua nhẹ.</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Sữa chua tách nước, có màu trắng sữa, có vị chua nhẹ.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Sữa chua đông tụ, có màu vàng ngà, có vị chua nhẹ.</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Sữa chua sủi bọt, có màu vàng ngà, có vị chua nhẹ.</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Virus được cấu tạo từ 2 thành phần chính gồm</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>lõi nucleic acid và vỏ ngoài.</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>vỏ ngoài và vỏ capsid.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>lõi nucleic acid và vỏ capsid.</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>gai glycoprotein và lõi nucleic acid.</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>3</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Chu trình nhân lên của virus gồm 5 giai đoạn theo trình tự là</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>hấp thụ → xâm nhập → lắp ráp → tổng hợp → giải phóng.</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>hấp thụ → xâm nhập → tổng hợp → giải phóng → lắp ráp.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>hấp thụ → lắp ráp → xâm nhập → tổng hợp → giải phóng.</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>hấp thụ → xâm nhập → tổng hợp → lắp ráp → giải phóng.</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>4</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Trong quá trình nhân lên của virus, giai đoạn có sự nhân lên của nucleic acid trong tế bào chủ là</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>hấp thụ.</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>xâm nhập.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>tổng hợp.</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>lắp ráp.</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>3</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Phát biểu nào sau đây là đúng khi nói về virus?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Virus có thể sống tự do hoặc kí sinh trên cơ thể sinh vật khác.</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Không thể nuôi virus trên môi trường nhân tạo như nuôi vi khuẩn.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Virus cũng có cấu tạo tế bào giống như các sinh vật khác.</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Virus có kích thước rất nhỏ nhưng vẫn lớn hơn vi khuẩn.</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>2</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Virus khác vi khuẩn ở điểm là</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>có kích thước lớn hơn.</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>có cấu tạo tế bào.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>có lối sống kí sinh nội bào bắt buộc.</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>có hình dạng và cấu trúc đa dạng.</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>3</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Các bệnh do virus thường có biểu hiện chung là</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>sốt cao, đau nhức các bộ phận cơ thể.</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>suy giảm hệ thống miễn dịch của cơ thể.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>sốt cao, tiêu chảy, đau họng.</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>tiêu chảy, đau nhức các bộ phận cơ thể.</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Virus gây hội chứng suy giảm miễn dịch mắc phải (AIDS) ở người là</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>HIV.</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>SARS-CoV-2.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Paramyxo virus.</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Aphtho type A.</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Các chủng virus cúm khác nhau về</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>chất cấu tạo lõi nucleic acid.</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>chất cấu tạo lớp vỏ ngoài.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>loại enzyme phiên mã ngược.</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>loại tổ hợp gai glycoprotein.</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>4</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Virus không gây bệnh theo cơ chế nào sau đây?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Cơ chế nhân lên kiểu sinh tan phá hủy các tế bào cơ thể và các mô.</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Cơ chế sản sinh các độc tố trong tế bào chủ làm biểu hiện triệu chứng bệnh.</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Cơ chế nhân lên kiểu tiềm tan gây đột biến gene dẫn đến ung thư.</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Cơ chế sản sinh các độc tố bên ngoài tế bào chủ làm biểu hiện triệu chứng bệnh.</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>4</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Virus không được sử dụng trong ứng dụng nào dưới đây?</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Chế tạo vaccine.</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Sản xuất thuốc trừ sâu.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Làm vector trong công nghệ di truyền.</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Sản xuất enzyme tự nhiên.</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>4</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Virus có vật chất di truyền là RNA dễ phát sinh các chủng đột biến hơn virus có vật</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>các virus RNA có khả năng tái tổ hợp với các virus RNA khác tạo ra loại virus mới.</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>các enzyme nhân bản RNA thường sao chép không chính xác và ít hoặc không có khả năng sửa chữa các sai sót.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>các virus RNA có vỏ protein linh hoạt, dễ bị biến tính trong môi trường nội bào của tế bào chủ.</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>các lõi nucleic acid của virus RNA thường có khả năng chủ động tạo ra những đột biến theo hướng tăng cường khả năng xâm nhập của virus.</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Triệu chứng điển hình của cây trồng bị nhiễm virus là</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>lá màu xanh đậm; thân cây mọc cao vống lên nhưng yếu và dễ đổ gãy.</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>lá bị xoăn; có những vết nâu, trắng hoặc vàng trên lá và quả; sinh trưởng chậm.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>lá có màu vàng đỏ; thân cây xuất hiện nhiều u bướu nhỏ.</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>sinh trưởng chậm; lá cây vàng héo rồi rụng; số lượng hoa và quả đều giảm.</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Vật trung gian truyền bệnh lùn xoắn lá ở lúa là</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>rầy nâu.</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ong mắt đỏ.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>ruồi giấm.</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>muỗi vằn.</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Dưới góc độ phòng bệnh, tại sao nên tránh tiếp xúc với các động vật hoang dã?</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Vì động vật hoang dã có thể là ổ chứa mầm bệnh truyền nhiễm.</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Vì động vật hoang dã có thể tấn công gây nguy hiểm cho con người.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Vì động vật hoang dã có thể làm biến đổi gene của con người.</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Vì động vật hoang dã có thể làm suy giảm hệ miễn dịch của con người.</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - kntt</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Đối với thụ thể bên trong tế bào, các phân tử tín hiệu</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>không thể liên kết với thụ thể.</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>liên kết với thụ thể ở bên ngoài tế bào.</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>liên kết với thụ thể màng.</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>đi qua màng và liên kết với thụ thể tạo thành phức hợp tín hiệu – thụ thể.</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>4</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Trong sự phân chia tế bào, các tế bào mới được tạo ra từ một tế bào</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>đều khác nhau.</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>đều khác nhau và một số giống tế bào mẹ.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>đều giống nhau và giống tế bào mẹ.</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>một số tế bào giống nhau và một số tế bào khác nhau.</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>3</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Hợp tử có bộ nhiễm sắc thể lưỡng bội</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>gấp đôi bộ nhiễm sắc thể đơn bội trong các giao tử.</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>gấp ba lần bộ nhiễm sắc thể đơn bội trong các giao tử.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>gấp bốn lần bộ nhiễm sắc thể đơn bội trong các giao tử.</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>bằng bộ nhiễm sắc thể đơn bội trong các giao tử.</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Hormone từ tế bào tuyến giáp được vận chuyển trong máu đến các tế bào cơ làm tăng cường hoạt động phiên mã, dịch mã và trao đổi chất ở các tế bào cơ. Sự truyền tin giữa tế bào tuyến giáp đến các tế bào cơ được thực hiện theo hình thức nào sau đây?</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Truyền tin cận tiết.</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Truyền tin nội tiết.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Truyền tin qua synapse.</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Truyền tin qua kết nối trực tiếp.</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>2</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Động vật có vú đầu tiên được nhân bản vô tính năm 1996 là</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>lợn Ỉ.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>bò Sahiwal.</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>cừu Dolly.</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>dê Beetal.</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>3</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Tế bào nào sau đây có tính toàn năng?</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Tế bào hồng cầu.</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Tế bào bạch cầu.</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Tế bào thần kinh.</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Tế bào hợp tử.</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>4</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Vi sinh vật có thể phân bố trong các loại môi trường là</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>môi trường đất, môi trường nước.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>môi trường trên cạn, môi trường sinh vật.</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>môi trường đất, môi trường nước, môi trường trên cạn.</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>môi trường đất, môi trường nước, môi trường trên cạn, môi trường sinh vật.</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>4</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Nguồn năng lượng cung cấp cho các hoạt động sống của vi khuẩn là</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ánh sáng.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>hóa học.</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>chất hữu cơ.</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>ánh sáng và hóa học.</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>4</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Nhóm sinh vật nào dưới đây thuộc nhóm vi sinh vật?</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Trùng roi, trùng giày, tảo đơn bào, rêu.</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Nấm men, trùng roi, tảo silic, vi khuẩn lactic.</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Trùng giày, rêu, giun, sán.</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Trùng giày, trùng biến hình, giun, sán.</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>2</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Phát biểu nào sau đây không đúng khi nói về vi sinh vật?</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Vi sinh vật là những cơ thể sống nhỏ bé mà mắt thường không nhìn thấy được.</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Vi sinh vật nhỏ bé nên quá trình trao đổi chất diễn ra mạnh.</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Phần lớn vi sinh vật là cơ thể đơn bào nhân sơ hoặc nhân thực.</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Vi sinh vật rất đa dạng nhưng phân bố của chúng rất hẹp.</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>4</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Sinh trưởng của vi sinh vật là</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>sự tăng lên về số lượng tế bào của quần thể vi sinh vật thông qua quá trình sinh sản.</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>sự tăng lên về số lượng tế bào của quần thể vi sinh vật thông qua quá trình nguyên phân.</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>sự tăng lên về số lượng tế bào của cơ thể vi sinh vật thông qua quá trình sinh sản.</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>sự tăng lên về số lượng tế bào của cơ thể vi sinh vật thông qua quá trình nguyên phân.</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Vi sinh vật nhân thực có thể sinh sản bằng các hình thức nào dưới đây?</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Phân đôi, nảy chồi, hình thành bào tử vô tính.</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Phân đôi, nảy chồi, hình thành bào tử hữu tính.</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Phân đôi, nảy chồi, hình thành bào tử vô tính và hữu tính.</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Hình thành bào tử vô tính và hữu tính.</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>3</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Để khắc phục hiện tượng mật độ tế bào vi khuẩn không tăng ở pha cân bằng có thể thực hiện biện pháp nào sau đây?</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Bổ sung thêm một lượng vi sinh vật giống thích hợp.</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Bổ sung thêm nguồn chất dinh dưỡng vào môi trường.</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Bổ sung thêm khí oxygen với nồng độ thích hợp.</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Bổ sung thêm khí nitrogen với nồng độ thích hợp.</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>2</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Vì sao một số chất hoá học như phenol, các kim loại nặng, alcohol thường dùng làm chất diệt khuẩn?</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Vì các chất này có thể gây biến tính và làm bất hoạt protein, phá hủy cấu trúc màng sinh chất,…</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Vì các chất này có thể tiêu diệt hoặc ức chế đặc hiệu sự sinh trưởng của một hoặc một vài nhóm vi sinh vật.</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Vì các chất này có thể gây biến đổi vật chất di truyền làm giảm khả năng thích nghi của vi sinh vật với môi trường.</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Vì các chất này có thể ngăn cản sự hấp thụ nước khiến các vi sinh vật bị chết do thiếu nước trầm trọng.</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Vi sinh vật nào sau đây quang hợp không thải O2?</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Vi khuẩn màu tía và màu lục.</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Vi khuẩn lam và vi tảo.</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Vi tảo và vi khuẩn màu tía.</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Vi khuẩn màu tía và vi tảo.</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Quá trình phân giải có vai trò là</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>hình thành các hợp chất đặc trưng để xây dựng và duy trì các hoạt động sống của tế bào.</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>hình thành năng lượng cung cấp cho quá trình tổng hợp và các hoạt động của tế bào.</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>hình thành nguyên liệu và năng lượng cung cấp cho quá trình tổng hợp và các hoạt động của tế bào.</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>hình thành các hợp chất tích lũy năng lượng để duy trì các hoạt động sống của tế bào.</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>3</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Con người ứng dụng quá trình tổng hợp các chất ức chế sự phát triển của các sinh vật khác ở vi sinh vật để</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>sản xuất dầu diesel sinh học.</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>sản xuất glutamic acid.</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>sản xuất nhựa hóa dầu.</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>sản xuất thuốc kháng sinh.</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>4</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Phát biểu nào sau đây là không đúng khi nói về quá trình phân giải ở vi sinh vật?</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Vi sinh vật có thể phân giải các hợp chất hữu cơ và chuyển hóa các chất vô cơ giúp khép kín vòng tuần hoàn vật chất trong tự nhiên.</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Con người có thể ứng dụng quá trình phân giải của vi sinh vật trong xử lí ô nhiễm môi trường, tạo ra các sản phẩm hữu ích khác.</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Khả năng phân giải của vi sinh vật trong tự nhiên là đa dạng và ngẫu nhiên nhưng luôn có hại cho con người.</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Vi sinh vật có khả năng phân giải làm hư hỏng thực phẩm, gây mất mĩ quan các vật dụng, đồ gỗ dùng xây dựng nhà cửa,…</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>3</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Trong quy trình sản xuất ethanol sinh học, người ta đã sử dụng vi sinh vật nào dưới đây để chuyển hóa đường thành ethanol?</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Nấm mốc Aspergillus niger.</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Vi khuẩn Bacillus thuringiensis.</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Nấm men Saccharomyces cerevisiae.</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Vi tảo Arthrospira platensis.</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>3</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Dạng sống không có cấu tạo tế bào, kích thước rất nhỏ, sống kí sinh bắt buộc trong tế bào của sinh vật là</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>vi khuẩn.</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>virus.</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>vi tảo.</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>vi nấm.</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>2</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Virus cố định trên bề mặt tế bào chủ nhờ mối liên kết đặc hiệu giữa thụ thể của virus và thụ thể của tế bào chủ là giai đoạn nào trong chu trình nhân lên của virus?</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Hấp phụ.</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Xâm nhập.</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Sinh tổng hợp.</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Lắp ráp.</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Cấu trúc đóng vai trò là thụ thể của virus có màng bọc là</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>vỏ capsid.</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>lông đuôi.</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>lõi nucleic acid.</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>các gai glycoprotein trên lớp màng phospholipid kép.</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>4</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Virus trần khác virus có màng bọc ở điểm là</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>có màng phospholipid kép bao bọc bên ngoài vỏ capsid.</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>chỉ có vật chất di truyền là DNA mạch thẳng, dạng kép.</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>chỉ có vật chất di truyền là RNA mạch vòng, dạng đơn.</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>có thụ thể là protein của vỏ capsid.</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>4</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Cây bị nhiễm virus thường có biểu hiện là</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>lá bị đốm vàng, đốm nâu, bị sọc hay vằn, bị xoăn và héo, bị úa vàng và rụng; thân còi cọc hoặc bị lùn.</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>lá bị đốm vàng, đốm nâu, bị sọc hay vằn, bị xoăn và héo, bị màu đỏ và rụng; thân cây mọc cao vống lên.</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>lá chuyển sang màu xanh đậm bất thường, bị xoăn, rụng sớm; thân cây còi cọc hoặc lùn, dễ bị đổ gãy.</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>lá bị đốm vàng, đốm nâu, bị nhỏ đi và dày lên bất thường, dễ rụng sớm; thân cây phát triển nhiều nhánh.</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Sự lây truyền của virus từ cơ thể mẹ sang cơ thể con thông qua quá trình mang thai là phương thức</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>lây truyền dọc.</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>lây truyền ngang.</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>lây truyền chéo.</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>lây truyền qua tiếp xúc trực tiếp.</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Miễn dịch đặc hiệu khác miễn dịch không đặc hiệu ở điểm là</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>được hình thành sau khi cơ thể tiếp xúc với mầm bệnh.</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>là phản ứng miễn dịch chung đối với tất cả các mầm bệnh.</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>giúp ngăn cản mầm bệnh xâm nhập vào tế bào và cơ thể.</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>được hình thành mà không cần yêu cầu tiếp xúc với mầm bệnh.</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Vì sao để hạn chế sự lây truyền của virus gây bệnh vàng lùn, lùn xoắn lá ở lúa, người ta thường phun thuốc diệt rầy nâu?</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Vì rầy nâu là tác nhân trực tiếp gây ra bệnh vàng lùn, lùn xoắn lá.</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Vì rầy nâu là vật chủ trung gian truyền virus gây bệnh vàng lùn, lùn xoắn lá.</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Vì rầy nâu hút nhựa cây khiến cây bị bệnh vàng lùn, lùn xoắn lá héo nhanh hơn.</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Vì rầy nâu hút nước của cây khiến cây bị bệnh vàng lùn, lùn xoắn lá héo nhanh hơn.</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>2</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Khi đưa chế phẩm vaccine vector phòng virus SARS – CoV – 2 vào cơ thể thì</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>gene đích sẽ không biểu hiện và không hình thành được kháng thể.</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>gene đích sẽ được biểu hiện và hình thành kháng thể kích thích cơ thể sản sinh kháng nguyên tương ứng.</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>gene đích sẽ được biểu hiện và hình thành kháng nguyên kích thích cơ thể sản sinh kháng thể tương ứng.</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>gene đích sẽ không biểu hiện và hình thành kháng thể kích thích cơ thể sản sinh kháng nguyên tương ứng.</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>3</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CD</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Hoạt động nào xảy ra trong pha G1 của kì trung gian?</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Sự tổng hợp thêm tế bào chất và bào quan, chuẩn bị các nguyên liệu để nhân đôi DNA, nhiễm sắc thể.</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Trung thể tự nhân đôi.</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>DNA tự nhân đôi.</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Nhiễm sắc thể tự nhân đôi.</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>1</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Các loại cây dược liệu nào thường được nhân giống bằng công nghệ nuôi cấy mô tế bào?</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Cây chuối sứ, cây dừa, cây dâu tây.</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Cây keo lai, bạch đàn, cà phê, trầm hương.</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Cây trầm hương, cây mía, cây cẩm lai.</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Cây đinh lăng, cây đẳng sâm, sâm Ngọc Linh.</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>4</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Đặc điểm của tế bào chuyên hóa là gì?</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Mang hệ gene giống nhau, có màng cellulose, có khả năng phân chia.</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Có tính toàn năng, có khả năng phân chia vô tính.</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Có tính toàn năng, đã phân hóa nhưng không mất khả năng biến đổi và có khả năng phản phân hóa.</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Có tính toàn năng, nếu được nuôi dưỡng trong môi trường thích hợp thì sẽ phân hóa thành cơ quan.</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>3</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Đặc điểm nào sau đây không đúng với vi sinh vật?</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Có kích thước nhỏ.</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Phần lớn có cấu tạo đơn bào.</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Đều có khả năng tự dưỡng.</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Sinh trưởng nhanh.</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>3</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Trong quá trình sinh tổng hợp ở vi sinh vật, protein được tổng hợp bằng cách nào?</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Kết hợp các nucleotide với nhau.</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Kết hợp giữa các amino acid với nhau.</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Kết hợp giữa acid béo và glycerol.</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Kết hợp các phân tử đường đơn với nhau.</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>2</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Đâu không phải là vai trò của gôm đối với vi sinh vật?</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Bảo vệ tế bào vi sinh vật khỏi bị khô.</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Lưu trữ và bảo quản thông tin di truyền.</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Ngăn cản sự tiếp xúc của vi sinh vật với virus.</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Là nguồn dự trữ carbon và năng lượng của vi sinh vật.</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>2</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Trình tự sắp xếp nào sau đây là đúng khi nói về các pha sinh trưởng của quần thể vi khuẩn trong nuôi cấy không liên tục?</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Pha tiềm phát → Pha lũy thừa → Pha cân bằng → Pha suy vong.</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Pha tiềm phát → Pha cân bằng → Pha lũy thừa → Pha suy vong.</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Pha suy vong → Pha tiềm phát → Pha lũy thừa → Pha cân bằng.</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Pha suy vong → Pha lũy thừa → Pha tiềm phát → Pha cân bằng.</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>1</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Công nghệ vi sinh vật là</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>lĩnh vực nghiên cứu, ứng dụng vi sinh vật trong sản xuất, chế biến các sản phẩm phục vụ đời sống con người.</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>lĩnh vực nghiên cứu, ứng dụng vi sinh vật trong sản xuất, chế biến các sản phẩm xử lí ô nhiễm môi trường.</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>lĩnh vực nghiên cứu, ứng dụng vi sinh vật trong sản xuất, chế biến các sản phẩm thuốc chữa bệnh cho người và động vật.</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>lĩnh vực nghiên cứu, ứng dụng vi sinh vật trong sản xuất, chế biến các loại đồ ăn, thức uống giàu giá trị dinh dưỡng.</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Vi sinh vật nào sau đây được ứng dụng để sản xuất phomat?</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Lactococcus lactis.</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Aspergillus oryzae.</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Bacillus thuringiensis.</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Saccharomyces cerevisiae.</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>1</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Dưa muối thành phẩm đạt yêu cầu không có biểu hiện nào sau đây?</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Có vị chua, giòn.</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Có mùi thơm.</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Có nhiều bọt khí.</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Có màu vàng.</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>3</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Sinh trưởng ở vi khuẩn cần được xem xét trên phạm vi quần thể vì</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>vi khuẩnhoàn toànkhông có sự thay đổi về kích thước và khối lượng.</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>khó nhận ra sự thay đổi về kích thước và khối lượng của tế bào vi khuẩn.</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>vi khuẩn có khả năng trao đổi chất, sinh trưởng và phát triển rất nhanh.</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>khó nhận ra sự tồn tại, phát triển của tế bào vi khuẩn trong môi trường tự nhiên.</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>2</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Đặc điểm nào sau đây đúng với sinh sản ở vi sinh vật nhân sơ?</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Chỉ có hình thức sinh sản vô tính.</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Chỉ có hình thức sinh sản hữu tính.</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Có cả 2 hình thức: sinh sản vô tính và sinh sản hữu tính.</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Chưa có hình thức sinh sản.</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>1</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Đâu không phải là ưu điểm của thuốc trừ sâu sinh học so với thuốc trừ sâu hóa học?</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Cho hiệu quả diệt trừ sâu hại nhanh chóng.</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>An toàn với sức khỏe con người và môi trường.</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Bảo vệ được sự cân bằng sinh học trong tự nhiên.</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Sản xuất khá đơn giản và có chi phí thấp.</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>1</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Vì sao có thể bảo quản thực phẩm bằng cách phơi khô, bảo quản lạnh, ngâm trong dung dịch đường?</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Vì vi sinh vật chỉ sinh độc tố gây hại trong những điều kiện môi trường khắc nghiệt.</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Vì vi sinh vật chỉ sinh ra độc tố trong giới hạn nhất định của các yếu tố môi trường.</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Vì vi sinh vật chỉ sinh trưởng trong những điều kiện môi trường khắc nghiệt.</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Vì vi sinh vật chỉ sinh trưởng trong giới hạn nhất định của các yếu tố môi trường.</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>4</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Các đơn vị cấu tạo nên vỏ capsid của virus là</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>capsomer.</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>glycoprotein.</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>glycerol.</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>nucleotide.</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>1</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Dựa vào lớp vỏ ngoài, virus được phân thành các nhóm gồm</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>virus trần và virus có vỏ ngoài.</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>virus có cấu trúc xoắn, virus có cấu trúc khối và virus có cấu trúc hỗn hợp.</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>virus DNA và virus RNA.</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>virus kí sinh ở vi khuẩn, virus kí sinh ở nấm, virus kí sinh ở thực vật, virus kí sinh ở động vật và người.</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>1</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Tại sao virus không thể nuôi trong môi trường tổng hợp như vi khuẩn?</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Vì virus có kích thước rất nhỏ.</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Vì virus có vật chất di truyền là RNA.</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Vì virus sống kí sinh nội bào bắt buộc.</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Vì virus không mẫn cảm với chất kháng sinh.</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
+        <v>3</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Vì sao mỗi loại virus chỉ xâm nhập vào tế bào của vật chủ nhất định?</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Vì mỗi loại virus chỉ xâm nhập được vào những tế bào của vật chủ có hệ gene tương thích với hệ gene của virus.</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Vì mỗi loại virus chỉ xâm nhập được vào những tế bào của vật chủ có màng sinh chất tương thích với vỏ capsid của virus.</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Vì mỗi loại virus chỉ xâm nhập được vào những tế bào của vật chủ có hình dạng tương thích với hình dạng của virus.</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Vì mỗi loại virus chỉ xâm nhập được vào những tế bào của vật chủ có thụ thể tương thích với phân tử bề mặt của virus.</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>4</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Dựa vào tính chất nào mà phage được dùng để làm vector trong sản xuất chế phẩm sinh học bằng công nghệ tái tổ hợp?</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Một số phage, chứa các đoạn gene không thật sự quan trọng, nếu cắt bỏ và thay bởi một đoạn gene khác thì quá trình nhân lên của chúng không bị ảnh hưởng.</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Phage có hệ gene là các phân tử RNA, có thể vận chuyển bất cứ gene nào vào tế bào vi khuẩn và luôn có khả năng nhân lên rất nhanh.</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Một số phage chứa các DNA dạng vòng có thể mang gene mong muốn vào tế bào vi khuẩn và có khả năng nhân lên rất nhanh.</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Phagen có hệ gene là các phân tử DNA đủ dài để có thể vận chuyển các gene mong muốn vào tế bào vi khuẩn mà không ảnh hưởng đến khả năng nhân lên của nó trong tế bào vật chủ.</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
+        <v>1</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Để tạo ra số lượng lớn virus trong sản xuất thuốc trừ sâu từ virus, người ta sử dụng phương pháp nào sau đây?</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Sử dụng thực vật làm vật chủ để nhân nhanh số lượng virus.</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Sử dụng sâu làm vật chủ để nhân nhanh số lượng virus.</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Sử dụng vi khuẩn làm vật chủ để nhân nhanh số lượng virus.</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Sử dụng môi trường tổng hợp nhân tạo để nhân nhanh số lượng virus.</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
+        <v>2</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Dựa trên cơ sở nào sau đây để có thể sử dụng virus để tạo giống cây trồng?</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Sử dụng virus làm vector chuyển gen mong muốn vào cây trồng.</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Sử dụng virus làm kháng nguyên tạo sức miễn dịch cho cây trồng.</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Sử dụng virus làm tác nhân gây đột biến hệ gene của cây trồng.</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Sử dụng virus làm tác nhân điều khiển sự tái bản gene của cây trồng.</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
+        <v>1</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Thành tựu nào sau đây không phải là ứng dụng của virus trong y học?</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Sản xuất vaccine để phòng các bệnh do virus gây ra.</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Sản xuất kháng sinh để điều trị bệnh nhiễm khuẩn.</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Sản xuất hormone insulin để điều trị bệnh tiểu đường.</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Sản xuất interferon để tăng cường khả năng miễn dịch cho cơ thể.</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
+        <v>2</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Sản phẩm sinh học nào sau đây được sản xuất nhờ ứng dụng virus?</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Đệm lót sinh học.</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Bio - EM.</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Thuốc trừ sâu Bt.</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Insulin.</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
+        <v>4</v>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Đâu không phải là ứng dụng của vi sinh vật trong thực tiễn?</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Xử lí rác thải.</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Tổng hợp chất kháng sinh.</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Sản xuất thuốc trừ sâu sinh học.</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Tạo ra máy đo đường huyết.</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>4</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Một người bị nhiễm SARS-CoV-2 hắt hơi làm các giọt tiết bắn ra và lây lan sang những người xung quanh khi họ hít phải. Đây là kiểu lây lan qua con đường nào?</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Đường tiêu hóa.</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Đường hô hấp.</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Đường bài tiết.</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Đường tình dục.</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>2</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Tế bào thực vật có vách cellulose nên</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>virus có thể dễ dàng xâm nhập vào tế bào thực vật.</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>virus có thể lây nhiễm như ở tế bào động vật.</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>virus không thể xâm nhập vào tế bào thực vật.</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>virus chỉ có thể lây nhiễm qua vết thương.</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>4</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Hình thức lây truyền nào sau đây không thuộc phương thức truyền dọc ở thực vật?</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Truyền qua phấn hoa.</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Truyền qua hạt giống.</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Truyền qua vết thương.</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Truyền qua nhân giống vô tính.</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>3</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Virus RNA có tỉ lệ đột biến cao hơn virus DNA vì</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>virus RNA không có khả năng tự sửa chữa khi sao chép.</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>virus RNA có khả năng nhân lên nhanh chóng hơn virus DNA.</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>virus RNA có khả năng lây nhiễm trên nhiều đối tượng vật chủ.</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>virus RNA không có khả năng chống lại sự bảo vệ của hệ miễn dịch.</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>1</v>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Cuoi ki II - CTST</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Ở người ( 2n = 46), số NST trong 1 tế bào tại kì giữa của nguyên phân là</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>2</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Ở người ( 2n = 46 ), số NST trong 1 tế bào ở kì sau của nguyên phân là</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>4</v>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Một loài thực vật có bộ NST lưỡng bội là 2n = 24. Một tế bào đang tiến hành quá trình phân bào nguyên phân, ở kì  sau có số NST trong tế bào là</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>24 NST đơn.</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>24 NST kép.</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>48 NST đơn.</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>48 NST kép.</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>3</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Kết quả quá trình giảm phân I là tạo ra 2 tế bào con, mỗi tế bào chứa</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>n NST đơn.</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>n NST kép.</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2n NST đơn.</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>2n NST kép.</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>2</v>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Sự trao đổi chéo giữa các NST trong cặp tương đồng xảy ra vào kỳ</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>đầu I.</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>giữa I.</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>sau I.</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>đầu II.</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>1</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Kết quả của quá trình giảm phân là từ 1 tế bào tạo ra</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>2 tế bào con, mỗi tế bào có 2n NST.</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2 tế bào con, mỗi tế bào có n NST.</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>4 tế bào con, mỗi tế bào có 2n NST.</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>4 tế bào con, mỗi tế bào có n NST.</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>4</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Quá trình giảm phân xảy ra ở</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>tế bào sinh dục .</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>tế bào sinh dưỡng.</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>hợp tử.</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>giao tử.</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>1</v>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Một nhóm tế bào sinh tinh tham gia quá trình giảm phân đã tạo ra 512 tinh trùng. Số tế bào sinh tinh là</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>4</v>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Ở gà có bộ NST 2n=78. Một tế bào sinh dục đực sơ khai nguyên phân liên tiếp một số lần, tất cả các tế bào con tạo thành đều tham gia giảm phân tạo giao tử. Tổng số NST đơn trong tất cả các giao tử là 19968. Tế bào sinh dục sơ khai đó đã nguyên phân với số lần là</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>1</v>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Hoạt động quan trọng nhất của NST trong nguyên phân là</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>sự tự nhân đôi và sự đóng xoắn.</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>sự phân li đồng đều về 2 cực của tế bào.</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>sự tự nhân đôi và sự phân li.</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>sự đóng xoắn và tháo xoắn</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>3</v>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Vi sinh vật quang tự dưỡng cần nguồn năng lượng và nguồn cacbon chủ yếu từ</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>ánh sáng và CO2.</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>ánh sáng và chất hữu cơ.</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>chất vô cơ và CO2.</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>chất hữu cơ.</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>1</v>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Vi sinh vật quang  dị dưỡng cần nguồn năng lượng và nguồn cacbon chủ yếu từ</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>ánh sáng và CO2.</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>ánh sáng và chất hữu cơ.</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>chất vô cơ và CO2.</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>chất hữu cơ.</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>2</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Vi sinh vật hoá tự dưỡng cần nguồn năng lượng và nguồn cacbon chủ yếu từ</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>ánh sáng và CO2.</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>ánh sáng và chất hữu cơ.</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>chất vô cơ và CO2.</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>chất hữu cơ.</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>3</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Việc muối chua rau quả là lợi dụng hoạt động của</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>nấm men rượu.</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>vi khuẩn mì chính.</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>nấm cúc đen.</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>vi khuẩn lactic.</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>4</v>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Việc làm tương, nước chấm là lợi dụng quá trình</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>lên men rượu.</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>lên men lactic.</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>phân giải polisacarit.</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>phân giải protein</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>4</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Đối với vi khuẩn lactic, nước rau quả khi muối chua là môi trường</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>tự nhiên.</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>tổng hợp.</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>bán tổng hợp.</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>không phải A, B, C</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>1</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Trong môi trường nuôi cấy không liên tục pha sinh trưởng nào của VSV có đặc điểm sinh trưởng với tốc độ lớn nhất, số lượng tb trong quần thể tăng lên rất nhanh:</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Pha tiềm phát</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Pha lũy thừa</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Pha cân bằng</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Pha suy vong</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>2</v>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Sau thời gian của một thế hệ Số tb trong quần thể biến đổi ntn?</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Giữ nguyên</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Tăng gấp đôi</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Tăng rất nhanh</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Giảm một nữa</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>2</v>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Nhận biết môi trường nuôi cấy liên tục của vi khuẩn người ta có thể dựa vào:</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Có pha suy vong thành phần của môi trường nuôi cấy liên tục luôn ổn định, vsv sẽ sinh trưởng liên tục, mật độ vsv tương đối ổn định</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Có pha suy vong thành phần của môi trường nuôi cấy liên tục thay đổi, vsv sẽ sinh trưởng liên tục, mật độ vsv tương đối ổn định</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Không có pha suy vong thành phần của môi trường nuôi cấy liên tục luôn bỗ sung, vsv sẽ sinh trưởng liên tục, mật độ vsv tương đối thay đổi</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Không có pha suy vong thành phần của môi trường nuôi cấy liên tục luôn ổn định, vsv ngừng trưởng , mật độ vsv tương đối ổn định</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>3</v>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Số tế bào ban đầu của quần thể 2500, sau 1 giờ số lượng tế bào là:( mỗi lần phân chia mất 10 phút)</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>160 000</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>320 000</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>80 000</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>120 000</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>1</v>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Phát biểu đúng khi nói về virut:</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Virus là cơ thể chưa có cấu tạo tế bào, cấu tạo đơn giản</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Virus là thực thể chưa có cấu tạo tế bào, cấu tạo đơn giản</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Virus là thực thể chưa có cấu tạo tế bào, cấu tạo đơn giản chỉ gồm một loại nu được bao bởi vỏ Pr</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Virus là cơ thể cấu tạo tế bào đơn giản</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>3</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Phát biểu nào sau đây là sai khi nói về miễn dịch:</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Miễn dịch là khả năng của cơ thể chống lại các tác nhân gây bệnh</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Miễn dịch tế bào có sự tham gia của các tb T độc</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Miễn dịch không đặc hiệu đóng vai trò chủ chủ lực</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Miễn dịch thể dịch là miễn dịch sản xuất ra kháng thể</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>3</v>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Ví dụ nào là miễn dịch không đặc hiệu</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Đại thực bào và bạch cầu trung tính giết chết VSV theo cơ chế thực bào</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>kháng thể sản xuất ra để đáp lại sự xâm nhập của kháng nguyên</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Tế bào T độc tiết ra protein độc làm tan tế bào nhiễm</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>kháng nguyên phản ứng đặc hiệu với kháng thể</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>1</v>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Ví dụ nào là miễn dịch thể dịch</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Đại thực bào và bạch cầu trung tính giết chết VSV theo cơ chế thực bào</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Kháng thể sản xuất ra để đáp lại sự xâm nhập của kháng nguyên</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Tế bào T độc tiết ra protein độc làm tan tế bào nhiễm</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Dịch axit của dạ dày phá hủy vi sinh vật mẫn cảm axit</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>3</v>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Bệnh nhân nhiễm HIV vẫn có thể sống bình thường trong gia đình và cộng đồng không nên kì thị vì:</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>giai đoạn không triệu chứng kéo dài</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>HIV không lây qua giao tiếp và sử dụng chung đồ dùng hằng ngày</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>HIV chỉ làm suy giảm miễn dịch</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>gồm 3 giai đoạn phát triển bệnh</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>2</v>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr"/>
+      <c r="J132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>HIV gây hội chứng suy giảm miễn dịch ở người do</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>chúng gây nên bệnh AIDS</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>chúng gây nên bệnh cơ hội</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>chúng có khả năng gây nhiễm và phá hủy một số tế bào của hệ thống miễn dịch</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>chúng dễ lây truyền</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
+        <v>3</v>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr"/>
+      <c r="J133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Theo thí nghiệm của Franken- Conrat, nếu lấy lõi ARN của chủng virut B và một nữa vỏ chủng A với một nữa vỏ chủng B tạo viruts lai , thì sau khi phân lập ta được virut:</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>chủng A</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Chủng B</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Virut lai có lõi ARN của chủng virut B và một nữa vỏ chủng A với một nữa vỏ chủng B</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Virut lai có lõi ARN của chủng virut A và một nữa vỏ chủng A với một nữa vỏ chủng B</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>2</v>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr"/>
+      <c r="J134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Ở VN có 3 bệnh sốt rất phổ biến do muỗi là vật trung gian truyền nhiễm gồm sốt rét (1), sốt xuất huyết (2), viêm não nhật bản (3)</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>1 và 2 do virut gây nên</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>1 và 3  do virut gây nên</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2 và 3 do virut gây nên</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>1,2,3 do virut gây nên</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>3</v>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Đơn vị cấu tạo nên vỏ capsit của Virut gọi là:</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>nucleocapsit</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>capsome</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>nucleoxom</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>glicoprotein</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>2</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr"/>
+      <c r="J136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Đặc điểm nào sau đây của virut:
+Có cấu tạo tế bào(1), chứa riboxom(2), chỉ chứa  ADN hoặc ANR(3),kí sinh nội bào (4)</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>1,2</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>2,3</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>3.4</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>1,4</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>3</v>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>Sinh 10</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Cuoi HKII</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr"/>
+      <c r="J137" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>